<commit_message>
preenchendo os outros campos da planilha de analise de ponto de funcao
</commit_message>
<xml_diff>
--- a/09-08/FIAPQualidProjSWAula12FerramentaFPAProfRJPManual1.xlsx
+++ b/09-08/FIAPQualidProjSWAula12FerramentaFPAProfRJPManual1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonrmlocal\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fiap\09-08\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AB4B61-CE7F-4E43-A5F8-6315950E6269}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0056953-E08C-4C0D-BB3D-2FED084DDFA0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="81">
   <si>
     <t>FERRAMENTA DE ESTIATIVA DE PONTOS DE SOFTWARE POR ANÁLISE DE PONTOS DE FUNÇÃO (FPA - FUNCTION POINT ANALYSIS)</t>
   </si>
@@ -192,22 +192,82 @@
     <t>cadastrar produtos</t>
   </si>
   <si>
-    <t>alteração de produtos</t>
-  </si>
-  <si>
     <t>pesquisa de produto por codigo ou nome</t>
   </si>
   <si>
     <t>exportação de dados dos produtos</t>
   </si>
   <si>
-    <t>api</t>
+    <t>arquivo de produto extraido</t>
   </si>
   <si>
-    <t>arquivode produto</t>
+    <t>alteração de preço de produto cadastrado</t>
   </si>
   <si>
-    <t>arquivo de produto extraido</t>
+    <t>arquivo de produto</t>
+  </si>
+  <si>
+    <t>CdProd</t>
+  </si>
+  <si>
+    <t>Codigo interno de identificação de um produto na loja</t>
+  </si>
+  <si>
+    <t>CdFrabic</t>
+  </si>
+  <si>
+    <t>Codigo de fabricação do produto</t>
+  </si>
+  <si>
+    <t>NmProd</t>
+  </si>
+  <si>
+    <t>Nome do produto</t>
+  </si>
+  <si>
+    <t>PreUnit</t>
+  </si>
+  <si>
+    <t>Preço Unitario</t>
+  </si>
+  <si>
+    <t>UniMedida</t>
+  </si>
+  <si>
+    <t>Tipos de unidade de medida (kg, litro, peça, etc)</t>
+  </si>
+  <si>
+    <t>DtExportação</t>
+  </si>
+  <si>
+    <t>Data de exportação</t>
+  </si>
+  <si>
+    <t>DtAltProduto</t>
+  </si>
+  <si>
+    <t>Data de alteração do produto</t>
+  </si>
+  <si>
+    <t>CdProd, CdFrabic, NmProd, PreUnit, UniMedida</t>
+  </si>
+  <si>
+    <t>CdProd, CdFrabic, NmProd, PreUnit, UniMedida, DtExportação</t>
+  </si>
+  <si>
+    <t>CdProd,NmProd, PreUnit, DtAltProduto</t>
+  </si>
+  <si>
+    <t>CdProd, CdFrabic, NmProd, PreUnit, UniMedida, DtAltProduto</t>
+  </si>
+  <si>
+    <t>INPUT: CdProd, CdFrabic, NmProd, PreUnit, UniMedida; OUTPUT: CdProd, CdFrabic, NmProd, PreUnit, UniMedida, DtExportacao</t>
+  </si>
+  <si>
+    <t>INPUT(1): arquivo de produto; OUTPUT(1): arquivo de produto extraido</t>
+  </si>
+  <si>
+    <t>Registro de produto</t>
   </si>
 </sst>
 </file>
@@ -1414,8 +1474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H240"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="E12" sqref="D12:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1498,82 +1558,136 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="31"/>
+      <c r="B9" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="31">
+        <v>1</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="31">
+        <v>5</v>
+      </c>
       <c r="G9" s="31"/>
       <c r="H9" s="31"/>
     </row>
-    <row r="10" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="34"/>
+        <v>58</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="34">
+        <v>1</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="34">
+        <v>4</v>
+      </c>
       <c r="G10" s="34"/>
       <c r="H10" s="34"/>
     </row>
     <row r="11" spans="1:8" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="34"/>
+        <v>55</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="34">
+        <v>1</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="34">
+        <v>6</v>
+      </c>
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
     </row>
-    <row r="12" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="32" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="34"/>
+        <v>56</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="34">
+        <v>2</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="34">
+        <v>11</v>
+      </c>
       <c r="G12" s="34"/>
       <c r="H12" s="34"/>
     </row>
-    <row r="13" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="33"/>
+        <v>59</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>80</v>
+      </c>
       <c r="D13" s="34"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="34"/>
+      <c r="E13" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="34">
+        <v>6</v>
+      </c>
       <c r="G13" s="34"/>
       <c r="H13" s="34"/>
     </row>
-    <row r="14" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="33"/>
+        <v>57</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>80</v>
+      </c>
       <c r="D14" s="34"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="34"/>
+      <c r="E14" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="34">
+        <v>6</v>
+      </c>
       <c r="G14" s="34"/>
       <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
-        <v>60</v>
-      </c>
+      <c r="A15" s="33"/>
       <c r="B15" s="34"/>
       <c r="C15" s="33"/>
       <c r="D15" s="34"/>
@@ -3880,7 +3994,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4046,7 +4160,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B765"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4069,32 +4185,60 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
+      <c r="A4" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="27"/>
+      <c r="A5" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="27"/>
+      <c r="A6" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
+      <c r="A7" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="27"/>
+      <c r="A8" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27"/>
+      <c r="A9" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27"/>
+      <c r="A10" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>

</xml_diff>